<commit_message>
added hint to execute tests on Linux and Mac as well
</commit_message>
<xml_diff>
--- a/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
+++ b/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Number</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Environment (OS + Version, Architecture, Java Version):</t>
-  </si>
-  <si>
-    <t>ARE start file: start.bat (start.sh - Linux)</t>
   </si>
   <si>
     <t>CAM_MOUSE_1</t>
@@ -311,11 +308,6 @@
 4. Select model file 'TestModelAutostart.acs' and click 'Open'</t>
   </si>
   <si>
-    <t>TestModelAutostart.acs
-ARE start file: start.bat (start.sh - Linux)
-Command shell: cmd.exe (xterm or similar - Linux)</t>
-  </si>
-  <si>
     <t>1. Open command shell in bin/ARE directory
 2. Execute 
 start.bat TestModelAutostart.acs
@@ -344,25 +336,36 @@
 2. The page must be loadable and return the currently deployed model in xml</t>
   </si>
   <si>
-    <t>1. Execute Test CAM_MOUSE_1
-2.Check and write down memory footprint (taskmanager windows, top on Linux)
-3. Watch memory foot print during 1 minute
-4. Check memory footprint again after 1h</t>
-  </si>
-  <si>
     <t>Test Camera Mouse, autostart and manual start of other models, test stability</t>
   </si>
   <si>
     <t xml:space="preserve">The camera mouse must still be functional (no frozen video frame, mouse cursor still moving according head movement)
 The memory footprint may increase over a short-term period (30sec.) due to Java garbage collection behaviour but must stay stable in average over 1h.
 </t>
+  </si>
+  <si>
+    <t>Execute tests on windows (7, 8), Linux (e.g. Ubuntu) and Mac OS X</t>
+  </si>
+  <si>
+    <t>ARE start file: start.bat (start.sh - Linux, Mac OS X)</t>
+  </si>
+  <si>
+    <t>TestModelAutostart.acs
+ARE start file: start.bat (start.sh - Linux, Mac OS X)
+Command shell: cmd.exe (xterm or similar - Linux, Mac OS X)</t>
+  </si>
+  <si>
+    <t>1. Execute Test CAM_MOUSE_1
+2.Check and write down memory footprint (taskmanager windows, top on Linux, Mac OS X)
+3. Watch memory foot print during 1 minute
+4. Check memory footprint again after 1h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +396,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -446,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -464,6 +475,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,7 +748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -744,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,12 +782,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>24</v>
@@ -815,34 +832,34 @@
     </row>
     <row r="7" spans="1:6" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
@@ -851,16 +868,16 @@
     </row>
     <row r="9" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>15</v>
@@ -869,16 +886,16 @@
     </row>
     <row r="10" spans="1:6" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>16</v>
@@ -887,16 +904,16 @@
     </row>
     <row r="11" spans="1:6" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>17</v>
@@ -905,16 +922,16 @@
     </row>
     <row r="12" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>19</v>
@@ -923,16 +940,16 @@
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>21</v>
@@ -941,73 +958,73 @@
     </row>
     <row r="14" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F17" s="5"/>
     </row>

</xml_diff>

<commit_message>
corrected test model and corresponding test cases
</commit_message>
<xml_diff>
--- a/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
+++ b/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Number</t>
   </si>
@@ -223,14 +223,6 @@
     <t>CAM_MOUSE_3</t>
   </si>
   <si>
-    <t>Test CAM_MOUSE_2</t>
-  </si>
-  <si>
-    <t>1. Execute test CAM_MOUSE_2
-2. Right click on ARE GUI background panel
-3. Click on 'start button'</t>
-  </si>
-  <si>
     <t>CAM_MOUSE_4</t>
   </si>
   <si>
@@ -241,12 +233,6 @@
   </si>
   <si>
     <t>CAM_MOUSE_5</t>
-  </si>
-  <si>
-    <t>1. Execute test CAM_MOUSE_1
-2. Right click on ARE GUI background panel
-3. Click on 'resume button'
-4. Click on 'stop button'</t>
   </si>
   <si>
     <t>CAM_MOUSE_6</t>
@@ -284,9 +270,6 @@
     <t>Test CAM_MOUSE_3</t>
   </si>
   <si>
-    <t>1. Execute Test CAM_MOUSE_2 by clicking 10 times onto 'Start' button (Play) as fast as possible</t>
-  </si>
-  <si>
     <t>CAM_MOUSE_8</t>
   </si>
   <si>
@@ -322,12 +305,6 @@
 </t>
   </si>
   <si>
-    <t>1. Open command shell in bin/ARE directory
-2. Execute 
-start.bat --webservice TestModelAutostart.acs
-./start.sh --webservice TestModelAutostart.acs</t>
-  </si>
-  <si>
     <t>1. The page must not be loadable (err_connection_refused)
 2. The page must not be loadable (err_connection_refused)</t>
   </si>
@@ -359,6 +336,29 @@
 2.Check and write down memory footprint (taskmanager windows, top on Linux, Mac OS X)
 3. Watch memory foot print during 1 minute
 4. Check memory footprint again after 1h</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_3
+2. Right click on ARE GUI background panel
+3. Click on 'start button'</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_1
+2. Right click on ARE GUI background panel
+3. Click on 'pause button'
+4. Click on 'stop button'</t>
+  </si>
+  <si>
+    <t>1. Execute Test CAM_MOUSE_1  by clicking 10 times onto 'Start' button (Play) as fast as possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open command shell in bin/ARE directory
+2. Execute 
+start.bat --webservice TestModelAutostart.acs
+./start.sh --webservice TestModelAutostart.acs
+3. Open http://localhost:8082/
+4. Open http://localhost:8081/rest/runtime/model
+</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +759,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,10 +787,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>24</v>
@@ -835,16 +835,16 @@
         <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -856,10 +856,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
@@ -886,16 +886,16 @@
     </row>
     <row r="10" spans="1:6" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>16</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="11" spans="1:6" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
@@ -913,7 +913,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>17</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="12" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -931,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>19</v>
@@ -940,16 +940,16 @@
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>21</v>
@@ -958,73 +958,73 @@
     </row>
     <row r="14" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="E15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F17" s="5"/>
     </row>

</xml_diff>

<commit_message>
fixed some wrong button label descriptions (resume button,...)
</commit_message>
<xml_diff>
--- a/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
+++ b/CameraInputModules/XFacetrackerLK/Tests/integrationTests/01_CameraMouse/Test_cases_CameraMouse.xlsx
@@ -150,9 +150,6 @@
     <t>Start model</t>
   </si>
   <si>
-    <t>Pause model/Resume model</t>
-  </si>
-  <si>
     <t>1. The selected model must be deployed and started successfully.
 2. CameraMouse: 
 The camera LED must be on and the camera frames be visible in a dedicated video frame window.
@@ -215,21 +212,10 @@
     <t>Test CAM_MOUSE_1</t>
   </si>
   <si>
-    <t>1. Execute test CAM_MOUSE_1
-2. Right click on ARE GUI background panel
-3. Click on 'stop button'</t>
-  </si>
-  <si>
     <t>CAM_MOUSE_3</t>
   </si>
   <si>
     <t>CAM_MOUSE_4</t>
-  </si>
-  <si>
-    <t>1. Execute test CAM_MOUSE_1
-2. Right click on ARE GUI background panel
-3. Click on 'resume button'
-4. Click on 'start button'</t>
   </si>
   <si>
     <t>CAM_MOUSE_5</t>
@@ -338,17 +324,6 @@
 4. Check memory footprint again after 1h</t>
   </si>
   <si>
-    <t>1. Execute test CAM_MOUSE_3
-2. Right click on ARE GUI background panel
-3. Click on 'start button'</t>
-  </si>
-  <si>
-    <t>1. Execute test CAM_MOUSE_1
-2. Right click on ARE GUI background panel
-3. Click on 'pause button'
-4. Click on 'stop button'</t>
-  </si>
-  <si>
     <t>1. Execute Test CAM_MOUSE_1  by clicking 10 times onto 'Start' button (Play) as fast as possible</t>
   </si>
   <si>
@@ -359,6 +334,31 @@
 3. Open http://localhost:8082/
 4. Open http://localhost:8081/rest/runtime/model
 </t>
+  </si>
+  <si>
+    <t>Pause model/Start model</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_3
+2. Right click on ARE GUI background panel
+3. Click on 'Start Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_1
+2. Right click on ARE GUI background panel
+3. Click on ''Stop Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_1
+2. Right click on ARE GUI background panel
+3. Click on 'Pause Model' button
+4. Click on 'Start Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test CAM_MOUSE_1
+2. Right click on ARE GUI background panel
+3. Click on 'Pause Model' button
+4. Click on ''Stop Model' button</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +759,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,10 +776,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
@@ -787,13 +787,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
@@ -804,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -832,199 +832,199 @@
     </row>
     <row r="7" spans="1:6" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F17" s="5"/>
     </row>

</xml_diff>